<commit_message>
commit 27 sept 2025
</commit_message>
<xml_diff>
--- a/saucedemo/Testdata/Book1.xlsx
+++ b/saucedemo/Testdata/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>standard_user</t>
   </si>
@@ -24,7 +24,13 @@
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>wrong_user</t>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,6 +390,22 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>